<commit_message>
Added final project files
</commit_message>
<xml_diff>
--- a/SLA Report Overview.xlsx
+++ b/SLA Report Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/1995914277468/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\IS\Quality Assurance\ACCESSIBILITY\SLA Monthly Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="367" documentId="13_ncr:1_{E75D683B-5AF3-42FE-9AE9-FE259D4BA44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108A299D-10F5-479E-972C-8EAA518FC7D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92D8337-C362-4349-89BA-E9AE6EA66144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7785" yWindow="3150" windowWidth="23220" windowHeight="15345" xr2:uid="{C020AC1A-066C-49E3-9B8D-19805A06CB89}"/>
+    <workbookView xWindow="12555" yWindow="2400" windowWidth="38700" windowHeight="15345" xr2:uid="{C020AC1A-066C-49E3-9B8D-19805A06CB89}"/>
   </bookViews>
   <sheets>
     <sheet name="SLA and Time Data" sheetId="1" r:id="rId1"/>
@@ -6972,7 +6972,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="9" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="9" bestFit="1" customWidth="1"/>

</xml_diff>